<commit_message>
I have changed the sample parageraph for word count
</commit_message>
<xml_diff>
--- a/keyWordDrivenArtifactID/src/test/java/testData/TestCase.xlsx
+++ b/keyWordDrivenArtifactID/src/test/java/testData/TestCase.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13620" windowHeight="5220" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="12390" windowHeight="4155" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="dataForLogin" sheetId="1" r:id="rId1"/>
     <sheet name="testSteps" sheetId="2" r:id="rId2"/>
     <sheet name="objectRepository" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
+  <oleSize ref="A1:F12"/>
 </workbook>
 </file>
 
@@ -211,8 +211,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,7 +348,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -380,27 +380,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -432,24 +414,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -625,16 +589,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B10" sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -642,7 +606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -650,7 +614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -658,7 +622,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -666,7 +630,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -674,7 +638,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -682,7 +646,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -696,14 +660,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
@@ -711,12 +675,12 @@
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="2" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -733,7 +697,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="5" customFormat="1">
       <c r="A3" s="5" t="s">
         <v>48</v>
       </c>
@@ -742,7 +706,7 @@
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>11</v>
@@ -757,7 +721,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>10</v>
@@ -772,7 +736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>10</v>
@@ -787,7 +751,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>15</v>
@@ -799,7 +763,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="5" customFormat="1">
       <c r="A8" s="6" t="s">
         <v>52</v>
       </c>
@@ -808,7 +772,7 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>11</v>
@@ -821,7 +785,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>10</v>
@@ -836,7 +800,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="5" customFormat="1">
       <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
@@ -845,7 +809,7 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>11</v>
@@ -860,7 +824,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
         <v>10</v>
@@ -875,7 +839,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
         <v>10</v>
@@ -890,7 +854,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
         <v>10</v>
@@ -905,7 +869,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
         <v>15</v>
@@ -917,7 +881,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="5" customFormat="1">
       <c r="A17" s="5" t="s">
         <v>50</v>
       </c>
@@ -926,7 +890,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
         <v>11</v>
@@ -941,7 +905,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
         <v>10</v>
@@ -956,7 +920,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="1"/>
       <c r="B20" s="2" t="s">
         <v>10</v>
@@ -971,7 +935,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="1"/>
       <c r="B21" s="2" t="s">
         <v>15</v>
@@ -983,7 +947,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="5" t="s">
         <v>51</v>
       </c>
@@ -992,7 +956,7 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="1"/>
       <c r="B23" s="2" t="s">
         <v>11</v>
@@ -1007,7 +971,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
         <v>10</v>
@@ -1022,7 +986,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
         <v>10</v>
@@ -1037,7 +1001,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
         <v>15</v>
@@ -1049,7 +1013,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
         <v>56</v>
       </c>
@@ -1058,7 +1022,7 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
         <v>11</v>
@@ -1073,7 +1037,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
         <v>10</v>
@@ -1088,7 +1052,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
         <v>15</v>
@@ -1101,7 +1065,7 @@
       </c>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
     </row>
@@ -1118,16 +1082,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -1135,7 +1099,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1143,7 +1107,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
@@ -1151,7 +1115,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1159,7 +1123,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
@@ -1167,7 +1131,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1175,7 +1139,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1183,7 +1147,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -1191,7 +1155,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -1199,7 +1163,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
@@ -1207,7 +1171,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>

</xml_diff>